<commit_message>
Mejoras en la presición
</commit_message>
<xml_diff>
--- a/Limpieza completa.xlsx
+++ b/Limpieza completa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UAEH\01 Proyecto terminal\Identificador_bots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE79421E-C82A-435E-96B3-10D3751D4FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC083F1-53BB-4EAA-943A-7AF8ADDAA73D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Humanos" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="461">
   <si>
     <t>645f0192ec00cbaed25d8dee</t>
   </si>
@@ -1218,9 +1218,6 @@
   </si>
   <si>
     <t>6461657d5b029997ce1fd195</t>
-  </si>
-  <si>
-    <t>Tiene más de 3000 vistas, pero solo 1 like, 1 comentario y 1 retuit</t>
   </si>
   <si>
     <t>64615bda5b029997ce1fcc51</t>
@@ -1906,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B241"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,10 +1914,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B1" t="s">
         <v>460</v>
-      </c>
-      <c r="B1" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1999,601 +1996,601 @@
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
+      <c r="A19" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>18</v>
+      <c r="A21" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>22</v>
+      <c r="A25" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>27</v>
+      <c r="A30" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>28</v>
+      <c r="A31" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>30</v>
+      <c r="A33" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>32</v>
+      <c r="A35" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>34</v>
+      <c r="A37" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>37</v>
+      <c r="A40" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>38</v>
+      <c r="A41" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>49</v>
+      <c r="A52" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>50</v>
+      <c r="A53" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>56</v>
+      <c r="A59" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>57</v>
+      <c r="A60" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>80</v>
+      <c r="A83" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>81</v>
+      <c r="A84" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>86</v>
+      <c r="A89" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>87</v>
+      <c r="A90" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>95</v>
+      <c r="A98" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>96</v>
+      <c r="A99" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>98</v>
+      <c r="A101" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
-        <v>127</v>
+      <c r="A130" s="4" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B133" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="4" t="s">
-        <v>132</v>
+      <c r="A134" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B135" t="s">
         <v>134</v>
@@ -2601,102 +2598,102 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="3" t="s">
-        <v>149</v>
+      <c r="A151" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="4" t="s">
-        <v>152</v>
+      <c r="A154" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B155" t="s">
         <v>154</v>
@@ -2704,231 +2701,216 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" s="3" t="s">
         <v>200</v>
       </c>
     </row>
@@ -3060,10 +3042,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F201"/>
+  <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3075,10 +3057,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B1" t="s">
         <v>460</v>
-      </c>
-      <c r="B1" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3717,10 +3699,10 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>167</v>
+        <v>331</v>
       </c>
       <c r="B121" t="s">
-        <v>306</v>
+        <v>332</v>
       </c>
       <c r="C121" t="s">
         <v>333</v>
@@ -3734,10 +3716,10 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B122" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C122" t="s">
         <v>337</v>
@@ -3751,39 +3733,39 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B123" t="s">
-        <v>336</v>
+        <v>306</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
-        <v>338</v>
+      <c r="A124" s="4" t="s">
+        <v>339</v>
       </c>
       <c r="B124" t="s">
-        <v>306</v>
+        <v>340</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
-        <v>339</v>
+      <c r="A125" s="3" t="s">
+        <v>341</v>
       </c>
       <c r="B125" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B126" t="s">
-        <v>342</v>
+        <v>299</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B127" t="s">
         <v>299</v>
@@ -3791,7 +3773,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B128" t="s">
         <v>299</v>
@@ -3799,31 +3781,31 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B129" t="s">
-        <v>299</v>
+        <v>347</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
-        <v>346</v>
+      <c r="A130" s="4" t="s">
+        <v>348</v>
       </c>
       <c r="B130" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="4" t="s">
-        <v>348</v>
+      <c r="A131" s="3" t="s">
+        <v>350</v>
       </c>
       <c r="B131" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B132" t="s">
         <v>299</v>
@@ -3831,20 +3813,20 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="B133" t="s">
-        <v>299</v>
+        <v>352</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
+      </c>
+      <c r="B134" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B135" t="s">
         <v>299</v>
@@ -3852,7 +3834,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B136" t="s">
         <v>299</v>
@@ -3860,23 +3842,23 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B137" t="s">
-        <v>299</v>
+        <v>357</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B138" t="s">
-        <v>357</v>
+        <v>299</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B139" t="s">
         <v>299</v>
@@ -3884,7 +3866,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B140" t="s">
         <v>299</v>
@@ -3892,7 +3874,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B141" t="s">
         <v>299</v>
@@ -3900,7 +3882,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B142" t="s">
         <v>299</v>
@@ -3908,7 +3890,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B143" t="s">
         <v>299</v>
@@ -3916,39 +3898,39 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B144" t="s">
-        <v>299</v>
+        <v>365</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B145" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B146" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B147" t="s">
-        <v>369</v>
+        <v>299</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B148" t="s">
         <v>299</v>
@@ -3956,39 +3938,39 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B149" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="3" t="s">
-        <v>372</v>
+      <c r="A150" s="4" t="s">
+        <v>373</v>
       </c>
       <c r="B150" t="s">
-        <v>299</v>
+        <v>374</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="4" t="s">
-        <v>373</v>
+      <c r="A151" s="7" t="s">
+        <v>375</v>
       </c>
       <c r="B151" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="7" t="s">
-        <v>375</v>
+      <c r="A152" s="3" t="s">
+        <v>377</v>
       </c>
       <c r="B152" t="s">
-        <v>376</v>
+        <v>299</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B153" t="s">
         <v>299</v>
@@ -3996,7 +3978,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B154" t="s">
         <v>299</v>
@@ -4004,7 +3986,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B155" t="s">
         <v>299</v>
@@ -4012,7 +3994,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B156" t="s">
         <v>299</v>
@@ -4020,7 +4002,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B157" t="s">
         <v>299</v>
@@ -4028,31 +4010,31 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B158" t="s">
-        <v>299</v>
+        <v>342</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B159" t="s">
-        <v>342</v>
+        <v>385</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B160" t="s">
-        <v>385</v>
+        <v>299</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B161" t="s">
         <v>299</v>
@@ -4060,23 +4042,23 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B162" t="s">
-        <v>299</v>
+        <v>389</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B163" t="s">
-        <v>389</v>
+        <v>299</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B164" t="s">
         <v>299</v>
@@ -4084,7 +4066,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B165" t="s">
         <v>299</v>
@@ -4092,7 +4074,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B166" t="s">
         <v>299</v>
@@ -4100,7 +4082,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B167" t="s">
         <v>299</v>
@@ -4108,7 +4090,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B168" t="s">
         <v>299</v>
@@ -4116,7 +4098,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B169" t="s">
         <v>299</v>
@@ -4124,44 +4106,44 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B170" t="s">
-        <v>299</v>
+        <v>398</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B171" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B172" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>400</v>
+        <v>402</v>
+      </c>
+      <c r="B173" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B174" t="s">
-        <v>402</v>
+        <v>299</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B175" t="s">
         <v>299</v>
@@ -4169,7 +4151,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B176" t="s">
         <v>299</v>
@@ -4177,7 +4159,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B177" t="s">
         <v>299</v>
@@ -4185,7 +4167,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B178" t="s">
         <v>299</v>
@@ -4193,7 +4175,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B179" t="s">
         <v>299</v>
@@ -4201,7 +4183,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B180" t="s">
         <v>299</v>
@@ -4209,7 +4191,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B181" t="s">
         <v>299</v>
@@ -4217,15 +4199,15 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B182" t="s">
-        <v>299</v>
+        <v>412</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B183" t="s">
         <v>299</v>
@@ -4233,15 +4215,15 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B184" t="s">
-        <v>413</v>
+        <v>299</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B185" t="s">
         <v>299</v>
@@ -4249,7 +4231,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B186" t="s">
         <v>299</v>
@@ -4257,7 +4239,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B187" t="s">
         <v>299</v>
@@ -4265,15 +4247,15 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B188" t="s">
-        <v>299</v>
+        <v>419</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="3" t="s">
-        <v>418</v>
+      <c r="A189" t="s">
+        <v>420</v>
       </c>
       <c r="B189" t="s">
         <v>299</v>
@@ -4281,15 +4263,15 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B190" t="s">
-        <v>420</v>
+        <v>299</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>421</v>
+      <c r="A191" s="3" t="s">
+        <v>422</v>
       </c>
       <c r="B191" t="s">
         <v>299</v>
@@ -4297,7 +4279,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B192" t="s">
         <v>299</v>
@@ -4305,7 +4287,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B193" t="s">
         <v>299</v>
@@ -4313,7 +4295,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B194" t="s">
         <v>299</v>
@@ -4321,7 +4303,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B195" t="s">
         <v>299</v>
@@ -4329,7 +4311,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B196" t="s">
         <v>299</v>
@@ -4337,7 +4319,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B197" t="s">
         <v>299</v>
@@ -4345,7 +4327,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B198" t="s">
         <v>299</v>
@@ -4353,25 +4335,9 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B199" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="B200" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="B201" t="s">
         <v>299</v>
       </c>
     </row>
@@ -4401,7 +4367,7 @@
         <v>269</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4414,7 +4380,7 @@
         <v>271</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4428,7 +4394,7 @@
         <v>273</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4436,7 +4402,7 @@
         <v>274</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4444,7 +4410,7 @@
         <v>275</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4452,7 +4418,7 @@
         <v>276</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4460,7 +4426,7 @@
         <v>277</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4473,7 +4439,7 @@
         <v>279</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4481,7 +4447,7 @@
         <v>280</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4489,7 +4455,7 @@
         <v>281</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -4497,7 +4463,7 @@
         <v>282</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -4510,7 +4476,7 @@
         <v>284</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4518,7 +4484,7 @@
         <v>285</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4526,7 +4492,7 @@
         <v>286</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4534,10 +4500,10 @@
         <v>287</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4545,10 +4511,10 @@
         <v>288</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>446</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4556,10 +4522,10 @@
         <v>289</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4567,7 +4533,7 @@
         <v>290</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4575,7 +4541,7 @@
         <v>291</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4583,10 +4549,10 @@
         <v>292</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="F24" t="s">
         <v>450</v>
-      </c>
-      <c r="F24" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4594,10 +4560,10 @@
         <v>293</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F25" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4605,10 +4571,10 @@
         <v>294</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="F26" t="s">
         <v>452</v>
-      </c>
-      <c r="F26" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4616,7 +4582,7 @@
         <v>295</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4629,7 +4595,7 @@
         <v>297</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4637,7 +4603,7 @@
         <v>298</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4645,23 +4611,23 @@
         <v>300</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B33" t="s">
         <v>456</v>
-      </c>
-      <c r="B33" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B34" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F34">
         <v>31</v>
@@ -4669,10 +4635,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B35" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>